<commit_message>
adição de novas colunas e nova lógica - irregulares
</commit_message>
<xml_diff>
--- a/inputs/0 - Expansão/0 - Monitoramento Form 4.xlsx
+++ b/inputs/0 - Expansão/0 - Monitoramento Form 4.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29101"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29103"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="13" documentId="11_3CCBCC9B137B889B01D7688C20DAE49124D5BAA3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1F33EA8F-70DE-4C91-91BF-148E95A796F5}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="11_3DCBCC9B130B0EE8B7FEB2AF72EBE1A8CC33A84E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E3050359-D3CB-47C5-8320-72E0E2D97FFC}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Resumo" sheetId="1" r:id="rId1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5541" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5557" uniqueCount="292">
   <si>
     <t>Categoria</t>
   </si>
@@ -904,6 +904,15 @@
   </si>
   <si>
     <t>03/07/2025</t>
+  </si>
+  <si>
+    <t>06/07/2025</t>
+  </si>
+  <si>
+    <t>07/07/2025</t>
+  </si>
+  <si>
+    <t>04/07/2025</t>
   </si>
   <si>
     <t>ESSE FORMULARIO POSSIVELMENTE ESTA INCORRETO POIS ESTA ADIANTADO</t>
@@ -4674,7 +4683,7 @@
       </c>
       <c r="G2" s="28">
         <f ca="1">COUNTIF(INDIRECT(G$1&amp;"!E2:E1000"),$A2)</f>
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="H2" s="28">
         <f ca="1">COUNTIF(INDIRECT(H$1&amp;"!E2:E1000"),$A2)</f>
@@ -4702,7 +4711,7 @@
       </c>
       <c r="N2" s="29">
         <f ca="1">SUM(B2:M2)</f>
-        <v>274</v>
+        <v>290</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="15.75" customHeight="1">
@@ -4731,7 +4740,7 @@
       </c>
       <c r="G3" s="30">
         <f ca="1">COUNTIF(INDIRECT(G$1&amp;"!E2:E1000"),$A3)</f>
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="H3" s="30">
         <f ca="1">COUNTIF(INDIRECT(H$1&amp;"!E2:E1000"),$A3)</f>
@@ -4759,7 +4768,7 @@
       </c>
       <c r="N3" s="31">
         <f ca="1">SUM(B3:M3)</f>
-        <v>42</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="15.75" customHeight="1">
@@ -6295,7 +6304,7 @@
         <v>25</v>
       </c>
       <c r="D49" s="13" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="E49" s="13"/>
       <c r="F49" s="13"/>
@@ -7831,7 +7840,7 @@
         <v>25</v>
       </c>
       <c r="D49" s="13" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="E49" s="13"/>
       <c r="F49" s="13"/>
@@ -9367,7 +9376,7 @@
         <v>25</v>
       </c>
       <c r="D49" s="13" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="E49" s="13"/>
       <c r="F49" s="13"/>
@@ -10903,7 +10912,7 @@
         <v>25</v>
       </c>
       <c r="D49" s="13" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="E49" s="13"/>
       <c r="F49" s="13"/>
@@ -12439,7 +12448,7 @@
         <v>25</v>
       </c>
       <c r="D49" s="13" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="E49" s="13"/>
       <c r="F49" s="13"/>
@@ -13975,7 +13984,7 @@
         <v>25</v>
       </c>
       <c r="D49" s="13" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="E49" s="13"/>
       <c r="F49" s="13"/>
@@ -14305,7 +14314,7 @@
         <v>88</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="G1" s="11" t="s">
         <v>89</v>
@@ -14322,16 +14331,16 @@
         <v>31</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="G2" s="13" t="s">
         <v>95</v>
@@ -14361,8 +14370,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:U70"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -14375,7 +14384,7 @@
     <col min="6" max="6" width="20.28515625" customWidth="1"/>
     <col min="7" max="7" width="21.28515625" customWidth="1"/>
     <col min="8" max="8" width="18.5703125" customWidth="1"/>
-    <col min="9" max="9" width="14.7109375" customWidth="1"/>
+    <col min="9" max="9" width="17.42578125" customWidth="1"/>
     <col min="10" max="10" width="16.28515625" customWidth="1"/>
     <col min="11" max="11" width="16.5703125" customWidth="1"/>
     <col min="12" max="12" width="17.28515625" customWidth="1"/>
@@ -15494,7 +15503,7 @@
         FALSE
     )
 )</f>
-        <v>Atrasado</v>
+        <v>Enviado</v>
       </c>
       <c r="J5" s="45" t="str">
         <f t="array" aca="1" ref="J5" ca="1">IF(
@@ -15799,7 +15808,7 @@
         FALSE
     )
 )</f>
-        <v>Atrasado</v>
+        <v>Enviado</v>
       </c>
       <c r="J6" s="45" t="str">
         <f t="array" aca="1" ref="J6" ca="1">IF(
@@ -16104,7 +16113,7 @@
         FALSE
     )
 )</f>
-        <v>Atrasado</v>
+        <v>Enviado</v>
       </c>
       <c r="J7" s="45" t="str">
         <f t="array" aca="1" ref="J7" ca="1">IF(
@@ -17061,7 +17070,7 @@
         FALSE
     )
 )</f>
-        <v>Atrasado</v>
+        <v>Enviado</v>
       </c>
       <c r="J12" s="45" t="str">
         <f t="array" aca="1" ref="J12" ca="1">IF(
@@ -20625,7 +20634,7 @@
         FALSE
     )
 )</f>
-        <v>Atrasado</v>
+        <v>Enviado</v>
       </c>
       <c r="J24" s="45" t="str">
         <f t="array" aca="1" ref="J24" ca="1">IF(
@@ -22754,7 +22763,7 @@
         FALSE
     )
 )</f>
-        <v>Atrasado</v>
+        <v>Enviado</v>
       </c>
       <c r="J33" s="45" t="str">
         <f t="array" aca="1" ref="J33" ca="1">IF(
@@ -23695,7 +23704,7 @@
         FALSE
     )
 )</f>
-        <v>Atrasado</v>
+        <v>Enviado</v>
       </c>
       <c r="J38" s="45" t="str">
         <f t="array" aca="1" ref="J38" ca="1">IF(
@@ -23992,7 +24001,7 @@
         FALSE
     )
 )</f>
-        <v>Atrasado</v>
+        <v>Enviado</v>
       </c>
       <c r="J39" s="45" t="str">
         <f t="array" aca="1" ref="J39" ca="1">IF(
@@ -24289,7 +24298,7 @@
         FALSE
     )
 )</f>
-        <v>Atrasado</v>
+        <v>Enviado</v>
       </c>
       <c r="J40" s="45" t="str">
         <f t="array" aca="1" ref="J40" ca="1">IF(
@@ -24933,7 +24942,7 @@
         FALSE
     )
 )</f>
-        <v>Atrasado</v>
+        <v>Enviado</v>
       </c>
       <c r="J44" s="45" t="str">
         <f t="array" aca="1" ref="J44" ca="1">IF(
@@ -25230,7 +25239,7 @@
         FALSE
     )
 )</f>
-        <v>Atrasado</v>
+        <v>Enviado</v>
       </c>
       <c r="J45" s="45" t="str">
         <f t="array" aca="1" ref="J45" ca="1">IF(
@@ -25527,7 +25536,7 @@
         FALSE
     )
 )</f>
-        <v>Atrasado</v>
+        <v>Enviado</v>
       </c>
       <c r="J46" s="45" t="str">
         <f t="array" aca="1" ref="J46" ca="1">IF(
@@ -27656,7 +27665,7 @@
         FALSE
     )
 )</f>
-        <v>Atrasado</v>
+        <v>Enviado</v>
       </c>
       <c r="J55" s="45" t="str">
         <f t="array" aca="1" ref="J55" ca="1">IF(
@@ -28844,7 +28853,7 @@
         FALSE
     )
 )</f>
-        <v>Atrasado</v>
+        <v>Enviado</v>
       </c>
       <c r="J59" s="45" t="str">
         <f t="array" aca="1" ref="J59" ca="1">IF(
@@ -29141,7 +29150,7 @@
         FALSE
     )
 )</f>
-        <v>Atrasado</v>
+        <v>Enviado</v>
       </c>
       <c r="J60" s="45" t="str">
         <f t="array" aca="1" ref="J60" ca="1">IF(
@@ -31270,7 +31279,7 @@
         FALSE
     )
 )</f>
-        <v>Atrasado</v>
+        <v>Enviado</v>
       </c>
       <c r="J69" s="45" t="str">
         <f t="array" aca="1" ref="J69" ca="1">IF(
@@ -31973,9 +31982,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:U70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E39" sqref="E39"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -48876,7 +48883,7 @@
         FALSE
     )
 )</f>
-        <v>Atrasado</v>
+        <v>Enviado</v>
       </c>
       <c r="J69" s="45" t="str">
         <f t="array" aca="1" ref="J69" ca="1">IF(
@@ -51308,7 +51315,7 @@
   <dimension ref="A1:K58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="3" topLeftCell="D26" activePane="topRight" state="frozen"/>
+      <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
       <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
@@ -54891,8 +54898,8 @@
   <dimension ref="A1:K58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="3" topLeftCell="D16" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F37" sqref="F37"/>
+      <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -56685,8 +56692,8 @@
   <dimension ref="A1:K58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="3" topLeftCell="D16" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B25" sqref="B25"/>
+      <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -58456,8 +58463,8 @@
   <dimension ref="A1:K58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="3" topLeftCell="D24" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H39" sqref="H39"/>
+      <pane xSplit="3" topLeftCell="D11" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -58469,7 +58476,7 @@
     <col min="5" max="5" width="13" customWidth="1"/>
     <col min="6" max="6" width="18" customWidth="1"/>
     <col min="7" max="7" width="27" customWidth="1"/>
-    <col min="8" max="8" width="83.85546875" customWidth="1"/>
+    <col min="8" max="8" width="83.140625" customWidth="1"/>
     <col min="9" max="9" width="34" customWidth="1"/>
     <col min="10" max="10" width="25" customWidth="1"/>
     <col min="11" max="11" width="26" customWidth="1"/>
@@ -58718,10 +58725,12 @@
       <c r="D9" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="E9" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="F9" s="13"/>
+      <c r="E9" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>281</v>
+      </c>
       <c r="G9" s="15" t="s">
         <v>95</v>
       </c>
@@ -58745,10 +58754,12 @@
       <c r="D10" s="13" t="s">
         <v>110</v>
       </c>
-      <c r="E10" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="F10" s="13"/>
+      <c r="E10" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" s="13" t="s">
+        <v>282</v>
+      </c>
       <c r="G10" s="15" t="s">
         <v>95</v>
       </c>
@@ -58965,10 +58976,12 @@
       <c r="D18" s="13" t="s">
         <v>120</v>
       </c>
-      <c r="E18" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="F18" s="13"/>
+      <c r="E18" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="F18" s="13" t="s">
+        <v>283</v>
+      </c>
       <c r="G18" s="15" t="s">
         <v>95</v>
       </c>
@@ -59017,10 +59030,12 @@
       <c r="D20" s="13" t="s">
         <v>123</v>
       </c>
-      <c r="E20" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="F20" s="13"/>
+      <c r="E20" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="F20" s="13" t="s">
+        <v>283</v>
+      </c>
       <c r="G20" s="15" t="s">
         <v>95</v>
       </c>
@@ -59179,10 +59194,12 @@
       <c r="D26" s="13" t="s">
         <v>130</v>
       </c>
-      <c r="E26" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="F26" s="13"/>
+      <c r="E26" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="F26" s="13" t="s">
+        <v>282</v>
+      </c>
       <c r="G26" s="15" t="s">
         <v>95</v>
       </c>
@@ -59206,10 +59223,12 @@
       <c r="D27" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="E27" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="F27" s="13"/>
+      <c r="E27" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="F27" s="13" t="s">
+        <v>283</v>
+      </c>
       <c r="G27" s="15" t="s">
         <v>95</v>
       </c>
@@ -59233,10 +59252,12 @@
       <c r="D28" s="13" t="s">
         <v>135</v>
       </c>
-      <c r="E28" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="F28" s="13"/>
+      <c r="E28" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="F28" s="13" t="s">
+        <v>282</v>
+      </c>
       <c r="G28" s="15" t="s">
         <v>95</v>
       </c>
@@ -59260,10 +59281,12 @@
       <c r="D29" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="E29" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="F29" s="13"/>
+      <c r="E29" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="F29" s="13" t="s">
+        <v>283</v>
+      </c>
       <c r="G29" s="15" t="s">
         <v>95</v>
       </c>
@@ -59426,10 +59449,12 @@
       <c r="D35" s="13" t="s">
         <v>189</v>
       </c>
-      <c r="E35" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="F35" s="13"/>
+      <c r="E35" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="F35" s="13" t="s">
+        <v>282</v>
+      </c>
       <c r="G35" s="15" t="s">
         <v>95</v>
       </c>
@@ -59453,10 +59478,12 @@
       <c r="D36" s="13" t="s">
         <v>143</v>
       </c>
-      <c r="E36" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="F36" s="13"/>
+      <c r="E36" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="F36" s="13" t="s">
+        <v>283</v>
+      </c>
       <c r="G36" s="15" t="s">
         <v>95</v>
       </c>
@@ -59480,10 +59507,12 @@
       <c r="D37" s="13" t="s">
         <v>144</v>
       </c>
-      <c r="E37" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="F37" s="13"/>
+      <c r="E37" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="F37" s="13" t="s">
+        <v>282</v>
+      </c>
       <c r="G37" s="15" t="s">
         <v>95</v>
       </c>
@@ -59546,7 +59575,7 @@
         <v>95</v>
       </c>
       <c r="H39" s="13" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="I39" s="13"/>
       <c r="J39" s="13" t="s">
@@ -59567,10 +59596,12 @@
       <c r="D40" s="13" t="s">
         <v>192</v>
       </c>
-      <c r="E40" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="F40" s="13"/>
+      <c r="E40" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="F40" s="13" t="s">
+        <v>282</v>
+      </c>
       <c r="G40" s="15" t="s">
         <v>95</v>
       </c>
@@ -59594,10 +59625,12 @@
       <c r="D41" s="13" t="s">
         <v>148</v>
       </c>
-      <c r="E41" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="F41" s="13"/>
+      <c r="E41" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="F41" s="13" t="s">
+        <v>282</v>
+      </c>
       <c r="G41" s="15" t="s">
         <v>95</v>
       </c>
@@ -59681,7 +59714,7 @@
         <v>14</v>
       </c>
       <c r="F44" s="13" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="G44" s="15" t="s">
         <v>95</v>
@@ -59710,7 +59743,7 @@
         <v>14</v>
       </c>
       <c r="F45" s="13" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="G45" s="15" t="s">
         <v>95</v>
@@ -59793,7 +59826,7 @@
         <v>14</v>
       </c>
       <c r="F48" s="13" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="G48" s="15" t="s">
         <v>95</v>
@@ -59816,7 +59849,7 @@
         <v>25</v>
       </c>
       <c r="D49" s="13" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="E49" s="26" t="s">
         <v>15</v>
@@ -59845,10 +59878,12 @@
       <c r="D50" s="13" t="s">
         <v>159</v>
       </c>
-      <c r="E50" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="F50" s="13"/>
+      <c r="E50" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="F50" s="13" t="s">
+        <v>282</v>
+      </c>
       <c r="G50" s="15" t="s">
         <v>95</v>
       </c>
@@ -60007,10 +60042,12 @@
       <c r="D56" s="13" t="s">
         <v>204</v>
       </c>
-      <c r="E56" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="F56" s="13"/>
+      <c r="E56" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="F56" s="13" t="s">
+        <v>283</v>
+      </c>
       <c r="G56" s="15" t="s">
         <v>95</v>
       </c>
@@ -60063,10 +60100,12 @@
       <c r="D58" s="13" t="s">
         <v>169</v>
       </c>
-      <c r="E58" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="F58" s="13"/>
+      <c r="E58" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="F58" s="13" t="s">
+        <v>282</v>
+      </c>
       <c r="G58" s="15" t="s">
         <v>95</v>
       </c>

</xml_diff>